<commit_message>
Fix Mining data: corrected total movement values from chart re-read
Revised total movement against y-axis gridlines (0,20,40,60,80):
- 2028: 41->42, 2030: 47.7->50, 2032: 57.8->60
- 2034: 68.8->75 (peak), 2036: 48->50, 2038: 49.5->55
- 2040: 45.5->45, 2042: 30.8->31, 2044: 17.4->18, 2048: 7.9->8
All ore/waste values recalculated from corrected totals + strip ratios
</commit_message>
<xml_diff>
--- a/Greenbushes_LoM_Analysis.xlsx
+++ b/Greenbushes_LoM_Analysis.xlsx
@@ -593,22 +593,22 @@
         <v>2028</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>10</v>
+        <v>10.2</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>31</v>
+        <v>31.8</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>3.1</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>24.4</v>
+        <v>24.3</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>75.59999999999999</v>
+        <v>75.7</v>
       </c>
     </row>
     <row r="7">
@@ -616,22 +616,22 @@
         <v>2030</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>9</v>
+        <v>9.4</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>38.7</v>
+        <v>40.6</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>47.7</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>4.3</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>18.9</v>
+        <v>18.8</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>81.09999999999999</v>
+        <v>81.2</v>
       </c>
     </row>
     <row r="8">
@@ -639,13 +639,13 @@
         <v>2032</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>8.5</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>49.3</v>
+        <v>51.2</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>57.8</v>
+        <v>60</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>5.8</v>
@@ -662,13 +662,13 @@
         <v>2034</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>63.3</v>
+        <v>69</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>68.8</v>
+        <v>75</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>11.5</v>
@@ -685,22 +685,22 @@
         <v>2036</v>
       </c>
       <c r="B10" s="4" t="n">
-        <v>8</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>40</v>
+        <v>41.7</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>5</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>16.7</v>
+        <v>16.6</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>83.3</v>
+        <v>83.40000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -708,13 +708,13 @@
         <v>2038</v>
       </c>
       <c r="B11" s="4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>40.5</v>
+        <v>45</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>49.5</v>
+        <v>55</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>4.5</v>
@@ -731,22 +731,22 @@
         <v>2040</v>
       </c>
       <c r="B12" s="4" t="n">
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>38.5</v>
+        <v>38.1</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>45.5</v>
+        <v>45</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>5.5</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>15.4</v>
+        <v>15.3</v>
       </c>
       <c r="G12" s="4" t="n">
-        <v>84.59999999999999</v>
+        <v>84.7</v>
       </c>
     </row>
     <row r="13">
@@ -757,19 +757,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>30.8</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>3.4</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>22.7</v>
+        <v>22.6</v>
       </c>
       <c r="G13" s="4" t="n">
-        <v>77.3</v>
+        <v>77.40000000000001</v>
       </c>
     </row>
     <row r="14">
@@ -777,22 +777,22 @@
         <v>2044</v>
       </c>
       <c r="B14" s="4" t="n">
-        <v>6</v>
+        <v>6.2</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>11.4</v>
+        <v>11.8</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>17.4</v>
+        <v>18</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>1.9</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>34.5</v>
+        <v>34.4</v>
       </c>
       <c r="G14" s="4" t="n">
-        <v>65.5</v>
+        <v>65.59999999999999</v>
       </c>
     </row>
     <row r="15">
@@ -826,19 +826,19 @@
         <v>4.4</v>
       </c>
       <c r="C16" s="4" t="n">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>7.9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>0.8</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>55.7</v>
+        <v>55</v>
       </c>
       <c r="G16" s="4" t="n">
-        <v>44.3</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17">
@@ -848,22 +848,22 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>89.40000000000001</v>
+        <v>92.2</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>379</v>
+        <v>395.8</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>468.4</v>
+        <v>488</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>19.1</v>
+        <v>18.9</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>80.90000000000001</v>
+        <v>81.09999999999999</v>
       </c>
     </row>
     <row r="19">
@@ -2173,13 +2173,13 @@
         <v>2028</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>10</v>
+        <v>10.2</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>31</v>
+        <v>31.8</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>3.1</v>
@@ -2202,13 +2202,13 @@
         <v>2030</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>9</v>
+        <v>9.4</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>38.7</v>
+        <v>40.6</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>47.7</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>4.3</v>
@@ -2231,13 +2231,13 @@
         <v>2032</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>8.5</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>49.3</v>
+        <v>51.2</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>57.8</v>
+        <v>60</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>5.8</v>
@@ -2260,13 +2260,13 @@
         <v>2034</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>63.3</v>
+        <v>69</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>68.8</v>
+        <v>75</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>11.5</v>
@@ -2289,13 +2289,13 @@
         <v>2036</v>
       </c>
       <c r="B10" s="4" t="n">
-        <v>8</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>40</v>
+        <v>41.7</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>5</v>
@@ -2318,13 +2318,13 @@
         <v>2038</v>
       </c>
       <c r="B11" s="4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>40.5</v>
+        <v>45</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>49.5</v>
+        <v>55</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>4.5</v>
@@ -2347,13 +2347,13 @@
         <v>2040</v>
       </c>
       <c r="B12" s="4" t="n">
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>38.5</v>
+        <v>38.1</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>45.5</v>
+        <v>45</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>5.5</v>
@@ -2379,10 +2379,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>30.8</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>3.4</v>
@@ -2405,13 +2405,13 @@
         <v>2044</v>
       </c>
       <c r="B14" s="4" t="n">
-        <v>6</v>
+        <v>6.2</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>11.4</v>
+        <v>11.8</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>17.4</v>
+        <v>18</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>1.9</v>
@@ -2466,10 +2466,10 @@
         <v>4.4</v>
       </c>
       <c r="C16" s="4" t="n">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>7.9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>0.8</v>
@@ -2615,7 +2615,7 @@
       </c>
       <c r="B5" s="8" t="inlineStr">
         <is>
-          <t>2034 - Total movement ~68.8 Mt with highest strip ratio of 11.5. This is a massive waste stripping campaign.</t>
+          <t>2034 - Total movement ~75.0 Mt with highest strip ratio of 11.5. This is a massive waste stripping campaign.</t>
         </is>
       </c>
     </row>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="B6" s="8" t="inlineStr">
         <is>
-          <t>89.4 Mt across even-year snapshots</t>
+          <t>92.2 Mt across even-year snapshots</t>
         </is>
       </c>
     </row>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="B7" s="8" t="inlineStr">
         <is>
-          <t>379.0 Mt across even-year snapshots</t>
+          <t>395.8 Mt across even-year snapshots</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B8" s="8" t="inlineStr">
         <is>
-          <t>4.24 (waste:ore) - Very high waste burden, especially in 2034</t>
+          <t>4.29 (waste:ore) - Very high waste burden, especially in 2034</t>
         </is>
       </c>
     </row>

</xml_diff>